<commit_message>
- remove CollectionLabel for now
</commit_message>
<xml_diff>
--- a/docs/Employment Data Bible.xlsx
+++ b/docs/Employment Data Bible.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="7580" yWindow="4260" windowWidth="25620" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>data/</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>e.g., computrabajo-ve-20121108.json</t>
-  </si>
-  <si>
-    <t>CollectionLabel</t>
-  </si>
-  <si>
-    <t>e.g., Run1, FullEndToEnd, etc.</t>
   </si>
   <si>
     <t>Filename</t>
@@ -205,8 +199,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,13 +227,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -560,7 +578,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -594,94 +612,86 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="E6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="E6" s="2" t="s">
+    <row r="8" spans="1:9">
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="D9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="E8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="F9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
+    <row r="10" spans="1:9">
+      <c r="E10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="E10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="F11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="4:9">
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="4:9">
       <c r="E18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="4:9">
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="4:9">
       <c r="E20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="4:9">
       <c r="E21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>